<commit_message>
Clean up day1 files
</commit_message>
<xml_diff>
--- a/day1/exercise1.xlsx
+++ b/day1/exercise1.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -397,7 +397,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4490-48C8-B74B-4C448B9FDECE}"/>
             </c:ext>
@@ -411,11 +411,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1310262928"/>
-        <c:axId val="1310261680"/>
+        <c:axId val="-1480925280"/>
+        <c:axId val="-1480919296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1310262928"/>
+        <c:axId val="-1480925280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -472,12 +472,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1310261680"/>
+        <c:crossAx val="-1480919296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1310261680"/>
+        <c:axId val="-1480919296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,7 +534,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1310262928"/>
+        <c:crossAx val="-1480925280"/>
         <c:crossesAt val="-1.5"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -584,7 +584,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -766,73 +766,73 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>6.9120300000946591</c:v>
+                  <c:v>-6.9119700000008768</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3120300000107923</c:v>
+                  <c:v>-6.3119700000058279</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.7120300000157433</c:v>
+                  <c:v>-5.7119700000107789</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.1120300000206953</c:v>
+                  <c:v>-5.1119700000157309</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.5120299999812374</c:v>
+                  <c:v>-4.5119700000206819</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.912030000030597</c:v>
+                  <c:v>-3.9119700000034281</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3120299999689347</c:v>
+                  <c:v>-3.3119699999861747</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.7120299999960906</c:v>
+                  <c:v>-2.7119699999911262</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.1120299999899395</c:v>
+                  <c:v>-2.1119699999960773</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.5120299999948903</c:v>
+                  <c:v>-1.5119699999899259</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.91202999999429035</c:v>
+                  <c:v>-0.91196999999487705</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.31203000000479264</c:v>
+                  <c:v>-0.31196999999982822</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.28797000000135853</c:v>
+                  <c:v>0.28803000000632295</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.88797000000195847</c:v>
+                  <c:v>0.88802999999026955</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-1.4879699999914562</c:v>
+                  <c:v>1.4880299999964206</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-2.0879699999976076</c:v>
+                  <c:v>2.0880299999914698</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-2.6879699999926565</c:v>
+                  <c:v>2.6880300000087232</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-3.2879699999988072</c:v>
+                  <c:v>3.2880299999815672</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-3.8879700000160606</c:v>
+                  <c:v>3.8880299999988206</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-4.4879699999889056</c:v>
+                  <c:v>4.48802999999387</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-5.0879699999839545</c:v>
+                  <c:v>5.0880299999889189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B92B-4FEE-BA8F-87A0B288FB30}"/>
             </c:ext>
@@ -846,11 +846,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1310262928"/>
-        <c:axId val="1310261680"/>
+        <c:axId val="-1480918752"/>
+        <c:axId val="-1480915488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1310262928"/>
+        <c:axId val="-1480918752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -907,12 +907,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1310261680"/>
+        <c:crossAx val="-1480915488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1310261680"/>
+        <c:axId val="-1480915488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -969,7 +969,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1310262928"/>
+        <c:crossAx val="-1480918752"/>
         <c:crossesAt val="-1.5"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2462,13 +2462,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -2493,20 +2493,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C5" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f>($C$2-C5)^2+($D$2-C5)^2+($E$2-C5)^2</f>
-        <v>2.4982579999999999</v>
+        <v>0.41025799999999996</v>
       </c>
       <c r="E5" s="1">
-        <f>(($C$2-C5+$D$7)^2+($D$2-C5+$D$7)^2+($E$2-C5+$D$7)^2-D5)/$D$7</f>
-        <v>-5.0879699999839545</v>
+        <f>(($C$2-C5-$D$7)^2+($D$2-C5-$D$7)^2+($E$2-C5-$D$7)^2-D5)/$D$7</f>
+        <v>-0.91196999998932593</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>2</v>
       </c>
@@ -2514,12 +2514,12 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <f>B32</f>
         <v>-1</v>
@@ -2540,296 +2540,296 @@
         <v>4.3222579999999997</v>
       </c>
       <c r="D10" s="1">
-        <f>(($C$2-B10+$D$7)^2+($D$2-B10+$D$7)^2+($E$2-B10+$D$7)^2-C10)/$D$7</f>
-        <v>6.9120300000946591</v>
+        <f>(($C$2-B10-$D$7)^2+($D$2-B10-$D$7)^2+($E$2-B10-$D$7)^2-C10)/$D$7</f>
+        <v>-6.9119700000008768</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
-        <f>B10+($B$33-$B$32)/20</f>
+        <f t="shared" ref="B11:B30" si="0">B10+($B$33-$B$32)/20</f>
         <v>-0.9</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" ref="C11:C30" si="0">($C$2-B11)^2+($D$2-B11)^2+($E$2-B11)^2</f>
+        <f t="shared" ref="C11:C30" si="1">($C$2-B11)^2+($D$2-B11)^2+($E$2-B11)^2</f>
         <v>3.6610580000000006</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" ref="D11:D30" si="1">(($C$2-B11+$D$7)^2+($D$2-B11+$D$7)^2+($E$2-B11+$D$7)^2-C11)/$D$7</f>
-        <v>6.3120300000107923</v>
+        <f t="shared" ref="D11:D30" si="2">(($C$2-B11-$D$7)^2+($D$2-B11-$D$7)^2+($E$2-B11-$D$7)^2-C11)/$D$7</f>
+        <v>-6.3119700000058279</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
-        <f>B11+($B$33-$B$32)/20</f>
+        <f t="shared" si="0"/>
         <v>-0.8</v>
       </c>
       <c r="C12" s="1">
+        <f t="shared" si="1"/>
+        <v>3.0598580000000002</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="2"/>
+        <v>-5.7119700000107789</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
         <f t="shared" si="0"/>
-        <v>3.0598580000000002</v>
-      </c>
-      <c r="D12" s="1">
+        <v>-0.70000000000000007</v>
+      </c>
+      <c r="C13" s="1">
         <f t="shared" si="1"/>
-        <v>5.7120300000157433</v>
+        <v>2.5186579999999998</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="2"/>
+        <v>-5.1119700000157309</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B13" s="1">
-        <f>B12+($B$33-$B$32)/20</f>
-        <v>-0.70000000000000007</v>
-      </c>
-      <c r="C13" s="1">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
         <f t="shared" si="0"/>
-        <v>2.5186579999999998</v>
-      </c>
-      <c r="D13" s="1">
+        <v>-0.60000000000000009</v>
+      </c>
+      <c r="C14" s="1">
         <f t="shared" si="1"/>
-        <v>5.1120300000206953</v>
+        <v>2.0374580000000004</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="2"/>
+        <v>-4.5119700000206819</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B14" s="1">
-        <f>B13+($B$33-$B$32)/20</f>
-        <v>-0.60000000000000009</v>
-      </c>
-      <c r="C14" s="1">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
         <f t="shared" si="0"/>
-        <v>2.0374580000000004</v>
-      </c>
-      <c r="D14" s="1">
+        <v>-0.50000000000000011</v>
+      </c>
+      <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>4.5120299999812374</v>
+        <v>1.6162580000000004</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="2"/>
+        <v>-3.9119700000034281</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B15" s="1">
-        <f>B14+($B$33-$B$32)/20</f>
-        <v>-0.50000000000000011</v>
-      </c>
-      <c r="C15" s="1">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
         <f t="shared" si="0"/>
-        <v>1.6162580000000004</v>
-      </c>
-      <c r="D15" s="1">
+        <v>-0.40000000000000013</v>
+      </c>
+      <c r="C16" s="1">
         <f t="shared" si="1"/>
-        <v>3.912030000030597</v>
+        <v>1.2550580000000005</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="2"/>
+        <v>-3.3119699999861747</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B16" s="1">
-        <f>B15+($B$33-$B$32)/20</f>
-        <v>-0.40000000000000013</v>
-      </c>
-      <c r="C16" s="1">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
         <f t="shared" si="0"/>
-        <v>1.2550580000000005</v>
-      </c>
-      <c r="D16" s="1">
+        <v>-0.30000000000000016</v>
+      </c>
+      <c r="C17" s="1">
         <f t="shared" si="1"/>
-        <v>3.3120299999689347</v>
+        <v>0.95385800000000032</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="2"/>
+        <v>-2.7119699999911262</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="1">
-        <f>B16+($B$33-$B$32)/20</f>
-        <v>-0.30000000000000016</v>
-      </c>
-      <c r="C17" s="1">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
         <f t="shared" si="0"/>
-        <v>0.95385800000000032</v>
-      </c>
-      <c r="D17" s="1">
+        <v>-0.20000000000000015</v>
+      </c>
+      <c r="C18" s="1">
         <f t="shared" si="1"/>
-        <v>2.7120299999960906</v>
+        <v>0.71265800000000035</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="2"/>
+        <v>-2.1119699999960773</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="1">
-        <f>B17+($B$33-$B$32)/20</f>
-        <v>-0.20000000000000015</v>
-      </c>
-      <c r="C18" s="1">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
         <f t="shared" si="0"/>
-        <v>0.71265800000000035</v>
-      </c>
-      <c r="D18" s="1">
+        <v>-0.10000000000000014</v>
+      </c>
+      <c r="C19" s="1">
         <f t="shared" si="1"/>
-        <v>2.1120299999899395</v>
+        <v>0.5314580000000001</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.5119699999899259</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="1">
-        <f>B18+($B$33-$B$32)/20</f>
-        <v>-0.10000000000000014</v>
-      </c>
-      <c r="C19" s="1">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
         <f t="shared" si="0"/>
-        <v>0.5314580000000001</v>
-      </c>
-      <c r="D19" s="1">
+        <v>-1.3877787807814457E-16</v>
+      </c>
+      <c r="C20" s="1">
         <f t="shared" si="1"/>
-        <v>1.5120299999948903</v>
+        <v>0.41025800000000007</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.91196999999487705</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="1">
-        <f>B19+($B$33-$B$32)/20</f>
-        <v>-1.3877787807814457E-16</v>
-      </c>
-      <c r="C20" s="1">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="1">
         <f t="shared" si="0"/>
-        <v>0.41025800000000007</v>
-      </c>
-      <c r="D20" s="1">
+        <v>9.9999999999999867E-2</v>
+      </c>
+      <c r="C21" s="1">
         <f t="shared" si="1"/>
-        <v>0.91202999999429035</v>
+        <v>0.34905799999999998</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.31196999999982822</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="1">
-        <f>B20+($B$33-$B$32)/20</f>
-        <v>9.9999999999999867E-2</v>
-      </c>
-      <c r="C21" s="1">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="1">
         <f t="shared" si="0"/>
-        <v>0.34905799999999998</v>
-      </c>
-      <c r="D21" s="1">
+        <v>0.19999999999999987</v>
+      </c>
+      <c r="C22" s="1">
         <f t="shared" si="1"/>
-        <v>0.31203000000479264</v>
+        <v>0.34785799999999989</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="2"/>
+        <v>0.28803000000632295</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="1">
-        <f>B21+($B$33-$B$32)/20</f>
-        <v>0.19999999999999987</v>
-      </c>
-      <c r="C22" s="1">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
         <f t="shared" si="0"/>
-        <v>0.34785799999999989</v>
-      </c>
-      <c r="D22" s="1">
+        <v>0.29999999999999988</v>
+      </c>
+      <c r="C23" s="1">
         <f t="shared" si="1"/>
-        <v>-0.28797000000135853</v>
+        <v>0.40665799999999985</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="2"/>
+        <v>0.88802999999026955</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="1">
-        <f>B22+($B$33-$B$32)/20</f>
-        <v>0.29999999999999988</v>
-      </c>
-      <c r="C23" s="1">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
         <f t="shared" si="0"/>
-        <v>0.40665799999999985</v>
-      </c>
-      <c r="D23" s="1">
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="C24" s="1">
         <f t="shared" si="1"/>
-        <v>-0.88797000000195847</v>
+        <v>0.52545799999999987</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="2"/>
+        <v>1.4880299999964206</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B24" s="1">
-        <f>B23+($B$33-$B$32)/20</f>
-        <v>0.39999999999999991</v>
-      </c>
-      <c r="C24" s="1">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
         <f t="shared" si="0"/>
-        <v>0.52545799999999987</v>
-      </c>
-      <c r="D24" s="1">
+        <v>0.49999999999999989</v>
+      </c>
+      <c r="C25" s="1">
         <f t="shared" si="1"/>
-        <v>-1.4879699999914562</v>
+        <v>0.70425799999999983</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="2"/>
+        <v>2.0880299999914698</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B25" s="1">
-        <f>B24+($B$33-$B$32)/20</f>
-        <v>0.49999999999999989</v>
-      </c>
-      <c r="C25" s="1">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="1">
         <f t="shared" si="0"/>
-        <v>0.70425799999999983</v>
-      </c>
-      <c r="D25" s="1">
+        <v>0.59999999999999987</v>
+      </c>
+      <c r="C26" s="1">
         <f t="shared" si="1"/>
-        <v>-2.0879699999976076</v>
+        <v>0.94305799999999962</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="2"/>
+        <v>2.6880300000087232</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="1">
-        <f>B25+($B$33-$B$32)/20</f>
-        <v>0.59999999999999987</v>
-      </c>
-      <c r="C26" s="1">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="1">
         <f t="shared" si="0"/>
-        <v>0.94305799999999962</v>
-      </c>
-      <c r="D26" s="1">
+        <v>0.69999999999999984</v>
+      </c>
+      <c r="C27" s="1">
         <f t="shared" si="1"/>
-        <v>-2.6879699999926565</v>
+        <v>1.2418579999999997</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="2"/>
+        <v>3.2880299999815672</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="1">
-        <f>B26+($B$33-$B$32)/20</f>
-        <v>0.69999999999999984</v>
-      </c>
-      <c r="C27" s="1">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="1">
         <f t="shared" si="0"/>
-        <v>1.2418579999999997</v>
-      </c>
-      <c r="D27" s="1">
+        <v>0.79999999999999982</v>
+      </c>
+      <c r="C28" s="1">
         <f t="shared" si="1"/>
-        <v>-3.2879699999988072</v>
+        <v>1.6006579999999995</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="2"/>
+        <v>3.8880299999988206</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="1">
-        <f>B27+($B$33-$B$32)/20</f>
-        <v>0.79999999999999982</v>
-      </c>
-      <c r="C28" s="1">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="1">
         <f t="shared" si="0"/>
-        <v>1.6006579999999995</v>
-      </c>
-      <c r="D28" s="1">
+        <v>0.8999999999999998</v>
+      </c>
+      <c r="C29" s="1">
         <f t="shared" si="1"/>
-        <v>-3.8879700000160606</v>
+        <v>2.0194579999999989</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="2"/>
+        <v>4.48802999999387</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B29" s="1">
-        <f>B28+($B$33-$B$32)/20</f>
-        <v>0.8999999999999998</v>
-      </c>
-      <c r="C29" s="1">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="1">
         <f t="shared" si="0"/>
-        <v>2.0194579999999989</v>
-      </c>
-      <c r="D29" s="1">
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="C30" s="1">
         <f t="shared" si="1"/>
-        <v>-4.4879699999889056</v>
+        <v>2.498257999999999</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="2"/>
+        <v>5.0880299999889189</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="1">
-        <f>B29+($B$33-$B$32)/20</f>
-        <v>0.99999999999999978</v>
-      </c>
-      <c r="C30" s="1">
-        <f t="shared" si="0"/>
-        <v>2.498257999999999</v>
-      </c>
-      <c r="D30" s="1">
-        <f t="shared" si="1"/>
-        <v>-5.0879699999839545</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>1</v>
       </c>

</xml_diff>